<commit_message>
modified brun doku, made some simulations in ISE
</commit_message>
<xml_diff>
--- a/VHDL_Brun/Logaritmik-Tabelle_LED-Fading.xlsx
+++ b/VHDL_Brun/Logaritmik-Tabelle_LED-Fading.xlsx
@@ -25,9 +25,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\ \=\&gt;\ 0\,"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -97,8 +94,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
@@ -107,6 +104,1703 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-CH"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1305161854768154"/>
+          <c:y val="4.6732747125143102E-2"/>
+          <c:w val="0.82892125984251963"/>
+          <c:h val="0.77262013643709704"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="50800"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$1:$A$256</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="256"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$1:$B$256</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="256"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6939446066310037E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4734295458518858E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.143400136661606</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19295284223808079</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24340857400488491</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29478378830463176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.34709524137291203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40035999480340789</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4545954211126001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50981920940588787</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56604937114695897</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6233042460323055</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.6816025079727881</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.74096317118420896</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.80140559638887754</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.86294949713018587</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.92561494620226337</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98942238219679945</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0543926161691748</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1205468384260706</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1879066254367747</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2564939468704319</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3263311727615466</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3974410808060553</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.4698468637903688</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.5435721371557907</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.6186409467007941</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.6950777764236522</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7729075565079986</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.8521556714539038</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.9328479683571371</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.0150107653393001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.0986708601315915</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.1838555388149925</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.2705925847197381</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.358910287486959</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.4488374522954692</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.5404034092566854</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.6336380229807674</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.7285717023170815</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.8252354102721684</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.9236606741084579</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.0238795956270117</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.1259248616376549</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.2298297546199164</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.3356281635782419</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.4433545950950348</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.553044184585112</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.6647327077552703</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.7784565922726747</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.8942529296458894</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.0121594873224282</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.1322147210067621</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.2544577872027949</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.3789285559849329</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.5056676240018545</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.6347163277172863</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.7661167568920488</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.8999117683118145</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.0361449997650132</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.174860884275482</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.3161046645944658</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.4599224079567463</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.6063610211056352</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.7554682655918139</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.9072927733509548</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.0618840625652179</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.2192925538138244</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.3795695865179152</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.5427674356851293</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.7089393289592962</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.8781394639808537</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.0504230260636449</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.2258462061938067</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.4044662193567028</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.5863413231978249</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7715308370237643</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.9600951611494368</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.1520957965978926</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.347595365159135</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.546657629814467</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.7493475155330422</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.9557311304474148</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>9.1658757874149739</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9.3798500259723099</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9.5977236346896664</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9.8195676739327471</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>10.045454499039366</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>10.275457783918435</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10.509652545078994</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>10.748115166097163</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>10.990923422528951</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>11.238156507277077</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>11.489895056420057</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>11.746221175511975</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>12.007218466361572</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>12.272972054299293</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>12.543568615941272</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>12.819096407459252</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>13.099645293365716</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>13.385306775823544</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>13.67617402448983</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>13.972341906903534</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>14.273907019426916</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>14.580967718750863</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>14.893624153974281</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>15.211978299268157</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>15.536133987134846</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>15.86619694227347</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>16.202274816062452</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>16.544477221670451</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>16.892915769807132</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>17.247704105125514</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>17.60895794328756</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>17.976795108705332</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>18.351335572969944</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>18.732701493980748</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>19.121017255787631</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>19.516409509159395</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>19.919007212891419</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>20.328941675866087</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>20.746346599879736</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>21.171358123249981</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>21.60411486521788</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>22.044757971159093</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>22.493431158619032</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>22.950280764186942</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>23.415455791224176</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>23.889107958462219</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>24.371391749486413</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>24.862464463121377</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>25.362486264734681</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>25.871620238475398</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>26.390032440464704</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>26.917891952955749</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>27.455370939480524</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>28.002644701001671</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>28.559891733087639</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>29.127293784129741</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>29.705035914620122</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>30.293306557509958</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>30.892297579667702</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>31.502204344457212</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>32.12322577545627</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>32.755564421336416</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>33.399426521924923</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>34.055022075470788</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>34.722564907136551</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>35.402272738738169</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>36.094367259755991</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>36.799074199639563</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>37.516623401430294</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>38.247248896725651</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>38.991188982009561</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>39.748686296373712</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>40.519987900655387</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>41.305345358017242</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>42.105014815995759</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>42.919257090044745</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>43.748337748601415</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>44.592527199702538</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>45.45210077917919</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>46.327338840458644</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>47.218526846002781</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>48.125955460412754</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>49.049920645230614</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>49.990723755468196</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>50.948671637895373</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>51.924076731119392</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>52.917257167487925</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>53.928536876849321</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>54.958245692203583</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>56.006719457278713</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>57.074300136067656</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>58.161335924361119</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>59.268181363313055</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>60.395197455075831</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>61.542751780542375</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>62.711218619234295</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>63.900979071374678</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>65.112421182185344</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>66.345940068449607</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>67.601938047381012</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>68.880824767840863</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>70.183017343946801</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>71.508940491116348</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>72.859026664589422</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>74.233716200475641</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>75.633457459371385</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>77.058706972594734</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>78.509929591084926</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>79.98759863701531</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>81.492196058169412</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>83.024212585130059</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>84.584147891333316</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>86.172510756038847</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>87.789819230270368</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>89.436600805780216</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>91.113392587092889</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>92.820741466683828</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>94.559204303350612</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>96.329348103834789</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>98.131750207753456</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>99.96699847590088</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>101.83569148198158</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>103.73843870783787</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>105.67586074223455</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>107.6485894832666</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>109.65726834445545</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>111.70255246460061</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>113.78510892145613</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>115.90561694930061</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>118.06476816047213</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>120.26326677094075</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>122.50182982999107</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>124.78118745409105</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>127.10208306502224</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>129.46527363235003</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>131.87152992031224</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>134.32163673920704</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>136.81639320136193</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>139.3566129817678</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>141.94312458346189</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>144.57677160774776</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>147.25841302933949</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>149.98892347651918</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>152.76919351640086</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>155.60012994539287</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>158.4826560849524</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>161.41771208273158</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>164.40625521920961</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>167.44926021991429</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>170.54771957333224</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>173.70264385461354</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>176.91506205517442</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>180.18602191830743</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>183.51659028090705</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>186.90785342142283</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>190.3609174141535</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>193.87690848999782</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>197.45697340377922</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>201.10227980826451</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>204.81401663499878</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>208.59339448208024</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>212.4416460090012</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>216.36002633868586</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>220.34981346685325</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>224.41230867884084</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>228.54883697402406</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>232.76074749797013</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>237.04941398246766</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>241.41623519357458</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>245.8626353878316</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>250.39006477678925</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="73081600"/>
+        <c:axId val="73075712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="73081600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="255"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Eingangswert</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73075712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="73075712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="255"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Ausgangswert</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73081600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>98698</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>144814</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>98698</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>32755</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,8 +2090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" topLeftCell="E219" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="M226" sqref="M226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2718,6 +4412,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>